<commit_message>
Add player's kills when killed some one in match
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Group.xlsx
+++ b/_Out/NFDataCfg/Excel/Group.xlsx
@@ -37,10 +37,10 @@
     <t>MatchStar</t>
   </si>
   <si>
-    <t>MatchDeathHero</t>
-  </si>
-  <si>
-    <t>MatchKillHero</t>
+    <t>MatchKilledHero</t>
+  </si>
+  <si>
+    <t>MatchBeKilledHero</t>
   </si>
   <si>
     <t>MatchGambleDiamond</t>
@@ -148,9 +148,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -168,22 +168,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,24 +181,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -227,55 +203,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -291,7 +220,92 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,20 +317,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -345,13 +345,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,19 +465,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,19 +489,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,121 +507,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,6 +651,78 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -672,54 +744,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -728,177 +752,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1344,7 +1344,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="$A11:$XFD11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
Added log for pvp module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Group.xlsx
+++ b/_Out/NFDataCfg/Excel/Group.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8805" activeTab="1"/>
+    <workbookView windowWidth="21000" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Property1-match" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>Id</t>
   </si>
@@ -37,10 +37,10 @@
     <t>MatchStar</t>
   </si>
   <si>
-    <t>MatchKilledHero</t>
-  </si>
-  <si>
-    <t>MatchBeKilledHero</t>
+    <t>MatchOpponentK</t>
+  </si>
+  <si>
+    <t>MatchOpponentD</t>
   </si>
   <si>
     <t>MatchGambleDiamond</t>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>MatchOpponentHeroStar3</t>
+  </si>
+  <si>
+    <t>MatchOpponentHeroHP1</t>
+  </si>
+  <si>
+    <t>MatchOpponentHeroHP2</t>
+  </si>
+  <si>
+    <t>MatchOpponentHeroHP3</t>
   </si>
   <si>
     <t>Type</t>
@@ -198,10 +207,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -222,42 +231,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -284,11 +257,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -300,9 +288,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,15 +305,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,7 +327,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -348,8 +334,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,8 +370,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,187 +411,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,8 +724,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,15 +735,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,13 +754,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,6 +784,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -794,168 +818,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1404,10 +1413,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W1" sqref="R1:W1"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1416,15 +1425,16 @@
     <col min="2" max="2" width="9.33333333333333" customWidth="1"/>
     <col min="3" max="5" width="19.125" customWidth="1"/>
     <col min="6" max="6" width="21.625" customWidth="1"/>
-    <col min="7" max="10" width="19.125" customWidth="1"/>
+    <col min="7" max="7" width="22.875" customWidth="1"/>
+    <col min="8" max="10" width="19.125" customWidth="1"/>
     <col min="11" max="11" width="20.375" customWidth="1"/>
     <col min="12" max="12" width="22.875" customWidth="1"/>
     <col min="13" max="13" width="20.375" customWidth="1"/>
     <col min="14" max="14" width="21.625" customWidth="1"/>
-    <col min="15" max="23" width="25.375" customWidth="1"/>
+    <col min="15" max="26" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" spans="1:23">
+    <row r="1" s="8" customFormat="1" spans="1:26">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1494,81 +1504,99 @@
       <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" s="9" customFormat="1" spans="1:23">
+    <row r="2" s="9" customFormat="1" spans="1:26">
       <c r="A2" s="14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="1" spans="1:23">
+    <row r="3" s="9" customFormat="1" spans="1:26">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1636,10 +1664,19 @@
       <c r="W3" s="3">
         <v>1</v>
       </c>
+      <c r="X3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" s="9" customFormat="1" spans="1:23">
+    <row r="4" s="9" customFormat="1" spans="1:26">
       <c r="A4" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1707,10 +1744,19 @@
       <c r="W4" s="3">
         <v>0</v>
       </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" s="9" customFormat="1" spans="1:23">
+    <row r="5" s="9" customFormat="1" spans="1:26">
       <c r="A5" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1778,10 +1824,19 @@
       <c r="W5" s="3">
         <v>0</v>
       </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" s="9" customFormat="1" spans="1:23">
+    <row r="6" s="9" customFormat="1" spans="1:26">
       <c r="A6" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1849,10 +1904,19 @@
       <c r="W6" s="3">
         <v>0</v>
       </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" s="10" customFormat="1" spans="1:23">
+    <row r="7" s="10" customFormat="1" spans="1:26">
       <c r="A7" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B7" s="10">
         <v>0</v>
@@ -1920,10 +1984,19 @@
       <c r="W7" s="10">
         <v>0</v>
       </c>
+      <c r="X7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" s="10" customFormat="1" spans="1:23">
+    <row r="8" s="10" customFormat="1" spans="1:26">
       <c r="A8" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10">
         <v>0</v>
@@ -1991,10 +2064,19 @@
       <c r="W8" s="10">
         <v>0</v>
       </c>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" s="10" customFormat="1" spans="1:23">
+    <row r="9" s="10" customFormat="1" spans="1:26">
       <c r="A9" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -2060,19 +2142,28 @@
         <v>0</v>
       </c>
       <c r="W9" s="10">
+        <v>0</v>
+      </c>
+      <c r="X9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="10" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A10" s="16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" s="17"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9 C7:C9 D7:D9 E7:E9 F7:F9 G7:G9 H7:H9 I7:I9 J7:J9 K7:K9 L7:L9 M7:M9 N7:N9 O7:O9 P7:P9 Q7:Q9 R7:R9 S7:S9 T7:T9 U7:U9 V7:V9 W7:W9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9 C7:C9 D7:D9 E7:E9 F7:F9 G7:G9 H7:H9 I7:I9 J7:J9 K7:K9 L7:L9 M7:M9 N7:N9 O7:O9 P7:P9 Q7:Q9 R7:R9 S7:S9 T7:T9 U7:U9 V7:V9 W7:W9 X7:X9 Y7:Y9 Z7:Z9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2087,8 +2178,8 @@
   <sheetPr/>
   <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2104,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2139,7 +2230,7 @@
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -2177,7 +2268,7 @@
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3">
         <v>18</v>
@@ -2215,7 +2306,7 @@
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2253,7 +2344,7 @@
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2291,7 +2382,7 @@
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2329,7 +2420,7 @@
     </row>
     <row r="7" spans="1:32">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -2367,7 +2458,7 @@
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2405,7 +2496,7 @@
     </row>
     <row r="9" spans="1:32">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2443,7 +2534,7 @@
     </row>
     <row r="10" ht="14.25" spans="1:32">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -2481,58 +2572,58 @@
     </row>
     <row r="11" spans="1:33">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -2552,58 +2643,58 @@
     </row>
     <row r="12" spans="1:33">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -2623,31 +2714,31 @@
     </row>
     <row r="13" spans="1:33">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>

</xml_diff>